<commit_message>
add term request information
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@83051 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ClinEpi_metadata.xlsx
+++ b/Load/src/ontology/ClinEpi_metadata.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="1160" windowWidth="32600" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="4500" windowWidth="29420" windowHeight="13800" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="terms" sheetId="1" r:id="rId1"/>
     <sheet name="issues" sheetId="3" r:id="rId2"/>
     <sheet name="notes" sheetId="2" r:id="rId3"/>
+    <sheet name="term request" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4848" uniqueCount="2027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5173" uniqueCount="2035">
   <si>
     <t>ID</t>
   </si>
@@ -6056,9 +6057,6 @@
     <t>ENVO?</t>
   </si>
   <si>
-    <t>OGMS</t>
-  </si>
-  <si>
     <t>OBI or OGMS</t>
   </si>
   <si>
@@ -6080,9 +6078,6 @@
     <t>OBI or OGMS?</t>
   </si>
   <si>
-    <t>OBI or DRON?</t>
-  </si>
-  <si>
     <t>ICO</t>
   </si>
   <si>
@@ -6102,13 +6097,43 @@
   </si>
   <si>
     <t>OGMS_0000096</t>
+  </si>
+  <si>
+    <t>OGMS or OBIB?</t>
+  </si>
+  <si>
+    <t>OBI or OMHI?</t>
+  </si>
+  <si>
+    <t>OMHI?</t>
+  </si>
+  <si>
+    <t>DRON?</t>
+  </si>
+  <si>
+    <t>OHMI</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/522</t>
+  </si>
+  <si>
+    <t>https://github.com/FoodOntology/foodon/issues/28</t>
+  </si>
+  <si>
+    <t>https://github.com/biobanking/biobanking/issues/37</t>
+  </si>
+  <si>
+    <t>https://github.com/ufbmi/OMRSE/issues/62</t>
+  </si>
+  <si>
+    <t>https://github.com/OHMI-ontology/OHMI/issues/1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6185,6 +6210,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6203,7 +6234,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="303">
+  <cellStyleXfs count="357">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6507,8 +6538,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6528,8 +6613,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="303">
+  <cellStyles count="357">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6681,6 +6768,33 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6832,6 +6946,33 @@
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7163,11 +7304,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I709"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D725" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C706" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E464" sqref="E464"/>
+      <selection pane="bottomRight" activeCell="G568" sqref="G568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7639,7 +7780,9 @@
       <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>1965</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="8" customFormat="1">
       <c r="A23" s="8" t="s">
@@ -7965,9 +8108,7 @@
       <c r="F36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>1967</v>
-      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
@@ -7988,9 +8129,7 @@
       <c r="F37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>1967</v>
-      </c>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
@@ -8009,9 +8148,7 @@
       <c r="F38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>1967</v>
-      </c>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
@@ -8032,9 +8169,7 @@
       <c r="F39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>1967</v>
-      </c>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
@@ -8124,9 +8259,6 @@
       <c r="F43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>1965</v>
-      </c>
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1">
       <c r="A44" s="2" t="s">
@@ -8147,9 +8279,6 @@
       <c r="F44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>1965</v>
-      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="2" t="s">
@@ -8650,9 +8779,7 @@
       <c r="F67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>2002</v>
-      </c>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="2" t="s">
@@ -8673,9 +8800,7 @@
       <c r="F68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G68" s="2" t="s">
-        <v>2002</v>
-      </c>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="2" t="s">
@@ -9062,9 +9187,7 @@
       <c r="F85" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G85" s="2" t="s">
-        <v>2002</v>
-      </c>
+      <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="2" t="s">
@@ -11208,7 +11331,7 @@
     </row>
     <row r="184" spans="1:9" s="9" customFormat="1">
       <c r="A184" s="9" t="s">
-        <v>823</v>
+        <v>1958</v>
       </c>
       <c r="B184" s="9" t="s">
         <v>390</v>
@@ -11216,22 +11339,19 @@
       <c r="C184" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="D184" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="E184" s="9" t="s">
-        <v>391</v>
+      <c r="D184" s="10" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E184" s="10" t="s">
+        <v>1639</v>
       </c>
       <c r="F184" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="H184" s="9" t="s">
-        <v>1975</v>
-      </c>
     </row>
     <row r="185" spans="1:9" s="9" customFormat="1">
       <c r="A185" s="9" t="s">
-        <v>571</v>
+        <v>823</v>
       </c>
       <c r="B185" s="9" t="s">
         <v>390</v>
@@ -11254,7 +11374,7 @@
     </row>
     <row r="186" spans="1:9" s="9" customFormat="1">
       <c r="A186" s="9" t="s">
-        <v>1958</v>
+        <v>571</v>
       </c>
       <c r="B186" s="9" t="s">
         <v>390</v>
@@ -11262,14 +11382,17 @@
       <c r="C186" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="D186" s="10" t="s">
-        <v>1639</v>
-      </c>
-      <c r="E186" s="10" t="s">
-        <v>1639</v>
+      <c r="D186" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>391</v>
       </c>
       <c r="F186" s="9" t="s">
         <v>93</v>
+      </c>
+      <c r="H186" s="9" t="s">
+        <v>1975</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -12573,7 +12696,7 @@
     </row>
     <row r="247" spans="1:8" s="3" customFormat="1">
       <c r="A247" s="3" t="s">
-        <v>1958</v>
+        <v>1127</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>594</v>
@@ -12581,25 +12704,22 @@
       <c r="C247" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="D247" s="11" t="s">
-        <v>1642</v>
-      </c>
-      <c r="E247" s="11" t="s">
-        <v>1642</v>
+      <c r="D247" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>949</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="G247" s="2" t="s">
         <v>1966</v>
       </c>
-      <c r="H247" s="3" t="s">
-        <v>1979</v>
-      </c>
     </row>
     <row r="248" spans="1:8" s="3" customFormat="1">
       <c r="A248" s="3" t="s">
-        <v>1127</v>
+        <v>1958</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>594</v>
@@ -12607,17 +12727,20 @@
       <c r="C248" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="D248" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="E248" s="3" t="s">
-        <v>949</v>
+      <c r="D248" s="11" t="s">
+        <v>1642</v>
+      </c>
+      <c r="E248" s="11" t="s">
+        <v>1642</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="G248" s="2" t="s">
         <v>1966</v>
+      </c>
+      <c r="H248" s="3" t="s">
+        <v>1979</v>
       </c>
     </row>
     <row r="249" spans="1:8" s="3" customFormat="1">
@@ -14136,7 +14259,7 @@
         <v>5</v>
       </c>
       <c r="G319" s="2" t="s">
-        <v>2011</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -14559,9 +14682,7 @@
       <c r="F339" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G339" s="2" t="s">
-        <v>2002</v>
-      </c>
+      <c r="G339" s="2"/>
     </row>
     <row r="340" spans="1:7">
       <c r="A340" s="2" t="s">
@@ -14582,9 +14703,7 @@
       <c r="F340" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G340" s="2" t="s">
-        <v>2002</v>
-      </c>
+      <c r="G340" s="2"/>
     </row>
     <row r="341" spans="1:7">
       <c r="A341" s="2" t="s">
@@ -14880,10 +14999,10 @@
       </c>
       <c r="G354" s="2"/>
       <c r="H354" s="8" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="I354" s="8" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="355" spans="1:9" s="3" customFormat="1">
@@ -14909,7 +15028,7 @@
         <v>1980</v>
       </c>
       <c r="H355" s="8" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="I355" s="8" t="s">
         <v>921</v>
@@ -14938,7 +15057,7 @@
         <v>1980</v>
       </c>
       <c r="H356" s="8" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="I356" s="8" t="s">
         <v>921</v>
@@ -14964,7 +15083,7 @@
         <v>1980</v>
       </c>
       <c r="H357" s="8" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="I357" s="8" t="s">
         <v>921</v>
@@ -15318,7 +15437,7 @@
         <v>5</v>
       </c>
       <c r="G374" s="2" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="375" spans="1:7">
@@ -15341,7 +15460,7 @@
         <v>5</v>
       </c>
       <c r="G375" s="2" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="376" spans="1:7">
@@ -15364,7 +15483,7 @@
         <v>5</v>
       </c>
       <c r="G376" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="377" spans="1:7">
@@ -15534,7 +15653,7 @@
         <v>5</v>
       </c>
       <c r="G384" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="385" spans="1:7">
@@ -15578,7 +15697,7 @@
         <v>93</v>
       </c>
       <c r="G386" s="2" t="s">
-        <v>2002</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="387" spans="1:7">
@@ -15601,7 +15720,7 @@
         <v>5</v>
       </c>
       <c r="G387" s="2" t="s">
-        <v>2002</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="388" spans="1:7">
@@ -15735,7 +15854,7 @@
         <v>5</v>
       </c>
       <c r="G393" s="2" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -15799,7 +15918,9 @@
       <c r="F396" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G396" s="2"/>
+      <c r="G396" s="2" t="s">
+        <v>2027</v>
+      </c>
     </row>
     <row r="397" spans="1:7">
       <c r="A397" s="2" t="s">
@@ -15820,7 +15941,9 @@
       <c r="F397" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G397" s="2"/>
+      <c r="G397" s="2" t="s">
+        <v>2027</v>
+      </c>
     </row>
     <row r="398" spans="1:7">
       <c r="A398" s="2" t="s">
@@ -15925,7 +16048,9 @@
       <c r="F402" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G402" s="2"/>
+      <c r="G402" s="2" t="s">
+        <v>2002</v>
+      </c>
     </row>
     <row r="403" spans="1:7">
       <c r="A403" s="2" t="s">
@@ -16122,7 +16247,7 @@
         <v>5</v>
       </c>
       <c r="G412" s="2" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="413" spans="1:7">
@@ -16223,7 +16348,7 @@
         <v>5</v>
       </c>
       <c r="G417" s="2" t="s">
-        <v>2019</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="418" spans="1:7">
@@ -16613,7 +16738,7 @@
         <v>93</v>
       </c>
       <c r="G437" s="2" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="438" spans="1:7">
@@ -16672,7 +16797,7 @@
         <v>5</v>
       </c>
       <c r="G440" s="2" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="441" spans="1:7">
@@ -16711,7 +16836,9 @@
       <c r="F442" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G442" s="2"/>
+      <c r="G442" s="2" t="s">
+        <v>2012</v>
+      </c>
     </row>
     <row r="443" spans="1:7">
       <c r="A443" s="2" t="s">
@@ -17187,7 +17314,7 @@
         <v>5</v>
       </c>
       <c r="G467" s="2" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="468" spans="1:7">
@@ -17208,7 +17335,7 @@
         <v>5</v>
       </c>
       <c r="G468" s="2" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="469" spans="1:7">
@@ -17229,7 +17356,7 @@
         <v>5</v>
       </c>
       <c r="G469" s="2" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="470" spans="1:7">
@@ -17250,7 +17377,7 @@
         <v>5</v>
       </c>
       <c r="G470" s="2" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="471" spans="1:7">
@@ -17290,7 +17417,7 @@
         <v>5</v>
       </c>
       <c r="G472" s="2" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="473" spans="1:7">
@@ -17435,7 +17562,7 @@
         <v>5</v>
       </c>
       <c r="G479" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="480" spans="1:7">
@@ -17479,7 +17606,7 @@
         <v>93</v>
       </c>
       <c r="G481" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="482" spans="1:7">
@@ -17663,7 +17790,7 @@
         <v>5</v>
       </c>
       <c r="G489" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="490" spans="1:7">
@@ -17707,7 +17834,7 @@
         <v>5</v>
       </c>
       <c r="G491" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="492" spans="1:7">
@@ -17730,7 +17857,7 @@
         <v>5</v>
       </c>
       <c r="G492" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="493" spans="1:7">
@@ -17753,7 +17880,7 @@
         <v>5</v>
       </c>
       <c r="G493" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="494" spans="1:7">
@@ -18028,7 +18155,7 @@
         <v>5</v>
       </c>
       <c r="G506" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="507" spans="1:7">
@@ -18051,7 +18178,7 @@
         <v>5</v>
       </c>
       <c r="G507" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="508" spans="1:7">
@@ -18139,7 +18266,7 @@
         <v>5</v>
       </c>
       <c r="G511" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="512" spans="1:7">
@@ -18225,7 +18352,7 @@
         <v>5</v>
       </c>
       <c r="G515" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="516" spans="1:7">
@@ -18290,7 +18417,7 @@
         <v>93</v>
       </c>
       <c r="G518" s="2" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="519" spans="1:7">
@@ -18313,7 +18440,7 @@
         <v>5</v>
       </c>
       <c r="G519" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="520" spans="1:7">
@@ -18336,7 +18463,7 @@
         <v>5</v>
       </c>
       <c r="G520" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="521" spans="1:7">
@@ -18571,7 +18698,7 @@
         <v>5</v>
       </c>
       <c r="G531" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="532" spans="1:7">
@@ -18594,7 +18721,7 @@
         <v>5</v>
       </c>
       <c r="G532" s="2" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="533" spans="1:7">
@@ -18617,7 +18744,7 @@
         <v>93</v>
       </c>
       <c r="G533" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="534" spans="1:7">
@@ -18640,7 +18767,7 @@
         <v>5</v>
       </c>
       <c r="G534" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="535" spans="1:7">
@@ -18663,7 +18790,7 @@
         <v>5</v>
       </c>
       <c r="G535" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="536" spans="1:7">
@@ -18686,7 +18813,7 @@
         <v>5</v>
       </c>
       <c r="G536" s="2" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="537" spans="1:7">
@@ -18709,7 +18836,7 @@
         <v>5</v>
       </c>
       <c r="G537" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="538" spans="1:7">
@@ -19051,7 +19178,7 @@
         <v>5</v>
       </c>
       <c r="G553" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="554" spans="1:7">
@@ -19095,7 +19222,7 @@
         <v>5</v>
       </c>
       <c r="G555" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="556" spans="1:7">
@@ -19118,7 +19245,7 @@
         <v>93</v>
       </c>
       <c r="G556" s="2" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="557" spans="1:7">
@@ -19206,7 +19333,7 @@
         <v>5</v>
       </c>
       <c r="G560" s="2" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="561" spans="1:7">
@@ -19355,7 +19482,7 @@
         <v>5</v>
       </c>
       <c r="G567" s="2" t="s">
-        <v>2002</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="568" spans="1:7">
@@ -20671,7 +20798,7 @@
     </row>
     <row r="633" spans="1:8" s="12" customFormat="1">
       <c r="A633" s="12" t="s">
-        <v>1283</v>
+        <v>1958</v>
       </c>
       <c r="B633" s="12" t="s">
         <v>1266</v>
@@ -20679,22 +20806,19 @@
       <c r="C633" s="12" t="s">
         <v>1258</v>
       </c>
-      <c r="D633" s="12" t="s">
-        <v>1152</v>
-      </c>
-      <c r="E633" s="12" t="s">
-        <v>1218</v>
+      <c r="D633" s="16" t="s">
+        <v>1646</v>
+      </c>
+      <c r="E633" s="16" t="s">
+        <v>1646</v>
       </c>
       <c r="F633" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="H633" s="12" t="s">
-        <v>1994</v>
       </c>
     </row>
     <row r="634" spans="1:8" s="12" customFormat="1">
       <c r="A634" s="12" t="s">
-        <v>1958</v>
+        <v>1283</v>
       </c>
       <c r="B634" s="12" t="s">
         <v>1266</v>
@@ -20702,19 +20826,22 @@
       <c r="C634" s="12" t="s">
         <v>1258</v>
       </c>
-      <c r="D634" s="16" t="s">
-        <v>1646</v>
-      </c>
-      <c r="E634" s="16" t="s">
-        <v>1646</v>
+      <c r="D634" s="12" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E634" s="12" t="s">
+        <v>1218</v>
       </c>
       <c r="F634" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="H634" s="12" t="s">
+        <v>1994</v>
       </c>
     </row>
     <row r="635" spans="1:8" s="14" customFormat="1">
       <c r="A635" s="14" t="s">
-        <v>1283</v>
+        <v>1958</v>
       </c>
       <c r="B635" s="14" t="s">
         <v>1267</v>
@@ -20722,22 +20849,19 @@
       <c r="C635" s="14" t="s">
         <v>1259</v>
       </c>
-      <c r="D635" s="14" t="s">
-        <v>1154</v>
-      </c>
-      <c r="E635" s="14" t="s">
-        <v>1220</v>
+      <c r="D635" s="15" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E635" s="15" t="s">
+        <v>1647</v>
       </c>
       <c r="F635" s="14" t="s">
         <v>5</v>
-      </c>
-      <c r="H635" s="15" t="s">
-        <v>1647</v>
       </c>
     </row>
     <row r="636" spans="1:8" s="14" customFormat="1">
       <c r="A636" s="14" t="s">
-        <v>1958</v>
+        <v>1283</v>
       </c>
       <c r="B636" s="14" t="s">
         <v>1267</v>
@@ -20745,14 +20869,17 @@
       <c r="C636" s="14" t="s">
         <v>1259</v>
       </c>
-      <c r="D636" s="15" t="s">
+      <c r="D636" s="14" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E636" s="14" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F636" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H636" s="15" t="s">
         <v>1647</v>
-      </c>
-      <c r="E636" s="15" t="s">
-        <v>1647</v>
-      </c>
-      <c r="F636" s="14" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="637" spans="1:8">
@@ -20898,7 +21025,7 @@
     </row>
     <row r="644" spans="1:8" s="12" customFormat="1">
       <c r="A644" s="12" t="s">
-        <v>1958</v>
+        <v>1127</v>
       </c>
       <c r="B644" s="12" t="s">
         <v>368</v>
@@ -20906,22 +21033,19 @@
       <c r="C644" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="D644" s="16" t="s">
-        <v>1649</v>
-      </c>
-      <c r="E644" s="16" t="s">
-        <v>1649</v>
+      <c r="D644" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="E644" s="12" t="s">
+        <v>371</v>
       </c>
       <c r="F644" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="H644" s="12" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="645" spans="1:8" s="12" customFormat="1">
       <c r="A645" s="12" t="s">
-        <v>1613</v>
+        <v>1958</v>
       </c>
       <c r="B645" s="12" t="s">
         <v>368</v>
@@ -20929,8 +21053,11 @@
       <c r="C645" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="D645" s="12" t="s">
-        <v>1400</v>
+      <c r="D645" s="16" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E645" s="16" t="s">
+        <v>1649</v>
       </c>
       <c r="F645" s="12" t="s">
         <v>5</v>
@@ -20941,7 +21068,7 @@
     </row>
     <row r="646" spans="1:8" s="12" customFormat="1">
       <c r="A646" s="12" t="s">
-        <v>1127</v>
+        <v>823</v>
       </c>
       <c r="B646" s="12" t="s">
         <v>368</v>
@@ -20953,7 +21080,7 @@
         <v>371</v>
       </c>
       <c r="E646" s="12" t="s">
-        <v>371</v>
+        <v>837</v>
       </c>
       <c r="F646" s="12" t="s">
         <v>5</v>
@@ -20961,7 +21088,7 @@
     </row>
     <row r="647" spans="1:8" s="12" customFormat="1">
       <c r="A647" s="12" t="s">
-        <v>823</v>
+        <v>1613</v>
       </c>
       <c r="B647" s="12" t="s">
         <v>368</v>
@@ -20970,13 +21097,13 @@
         <v>370</v>
       </c>
       <c r="D647" s="12" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F647" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H647" s="12" t="s">
         <v>371</v>
-      </c>
-      <c r="E647" s="12" t="s">
-        <v>837</v>
-      </c>
-      <c r="F647" s="12" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="648" spans="1:8" s="12" customFormat="1">
@@ -21186,7 +21313,7 @@
     </row>
     <row r="658" spans="1:8" s="12" customFormat="1">
       <c r="A658" s="12" t="s">
-        <v>1283</v>
+        <v>1127</v>
       </c>
       <c r="B658" s="12" t="s">
         <v>90</v>
@@ -21195,21 +21322,18 @@
         <v>92</v>
       </c>
       <c r="D658" s="12" t="s">
-        <v>1165</v>
+        <v>91</v>
       </c>
       <c r="E658" s="12" t="s">
-        <v>1165</v>
+        <v>91</v>
       </c>
       <c r="F658" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H658" s="12" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="659" spans="1:8" s="12" customFormat="1">
       <c r="A659" s="12" t="s">
-        <v>1127</v>
+        <v>1283</v>
       </c>
       <c r="B659" s="12" t="s">
         <v>90</v>
@@ -21218,13 +21342,16 @@
         <v>92</v>
       </c>
       <c r="D659" s="12" t="s">
-        <v>91</v>
+        <v>1165</v>
       </c>
       <c r="E659" s="12" t="s">
-        <v>91</v>
+        <v>1165</v>
       </c>
       <c r="F659" s="12" t="s">
         <v>93</v>
+      </c>
+      <c r="H659" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="660" spans="1:8" s="12" customFormat="1">
@@ -21292,7 +21419,7 @@
     </row>
     <row r="663" spans="1:8" s="14" customFormat="1">
       <c r="A663" s="14" t="s">
-        <v>1283</v>
+        <v>1958</v>
       </c>
       <c r="B663" s="14" t="s">
         <v>431</v>
@@ -21300,22 +21427,19 @@
       <c r="C663" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="D663" s="14" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E663" s="14" t="s">
-        <v>1221</v>
+      <c r="D663" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="E663" s="15" t="s">
+        <v>432</v>
       </c>
       <c r="F663" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H663" s="14" t="s">
-        <v>1996</v>
+        <v>93</v>
       </c>
     </row>
     <row r="664" spans="1:8" s="14" customFormat="1">
       <c r="A664" s="14" t="s">
-        <v>1958</v>
+        <v>1283</v>
       </c>
       <c r="B664" s="14" t="s">
         <v>431</v>
@@ -21323,14 +21447,17 @@
       <c r="C664" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="D664" s="15" t="s">
-        <v>432</v>
-      </c>
-      <c r="E664" s="15" t="s">
-        <v>432</v>
+      <c r="D664" s="14" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E664" s="14" t="s">
+        <v>1221</v>
       </c>
       <c r="F664" s="14" t="s">
-        <v>93</v>
+        <v>5</v>
+      </c>
+      <c r="H664" s="14" t="s">
+        <v>1996</v>
       </c>
     </row>
     <row r="665" spans="1:8" s="14" customFormat="1">
@@ -21501,7 +21628,7 @@
     </row>
     <row r="673" spans="1:8" s="9" customFormat="1">
       <c r="A673" s="9" t="s">
-        <v>1613</v>
+        <v>1127</v>
       </c>
       <c r="B673" s="9" t="s">
         <v>143</v>
@@ -21510,18 +21637,18 @@
         <v>145</v>
       </c>
       <c r="D673" s="9" t="s">
-        <v>1419</v>
+        <v>146</v>
+      </c>
+      <c r="E673" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F673" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="H673" s="9" t="s">
-        <v>1998</v>
       </c>
     </row>
     <row r="674" spans="1:8" s="9" customFormat="1">
       <c r="A674" s="9" t="s">
-        <v>1127</v>
+        <v>1958</v>
       </c>
       <c r="B674" s="9" t="s">
         <v>143</v>
@@ -21529,10 +21656,10 @@
       <c r="C674" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D674" s="9" t="s">
+      <c r="D674" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E674" s="9" t="s">
+      <c r="E674" s="10" t="s">
         <v>146</v>
       </c>
       <c r="F674" s="9" t="s">
@@ -21541,7 +21668,7 @@
     </row>
     <row r="675" spans="1:8" s="9" customFormat="1">
       <c r="A675" s="9" t="s">
-        <v>1958</v>
+        <v>1283</v>
       </c>
       <c r="B675" s="9" t="s">
         <v>143</v>
@@ -21549,11 +21676,11 @@
       <c r="C675" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D675" s="10" t="s">
-        <v>146</v>
+      <c r="D675" s="9" t="s">
+        <v>1150</v>
       </c>
       <c r="E675" s="10" t="s">
-        <v>146</v>
+        <v>1217</v>
       </c>
       <c r="F675" s="9" t="s">
         <v>5</v>
@@ -21561,7 +21688,7 @@
     </row>
     <row r="676" spans="1:8" s="9" customFormat="1">
       <c r="A676" s="9" t="s">
-        <v>1283</v>
+        <v>823</v>
       </c>
       <c r="B676" s="9" t="s">
         <v>143</v>
@@ -21570,10 +21697,10 @@
         <v>145</v>
       </c>
       <c r="D676" s="9" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E676" s="10" t="s">
-        <v>1217</v>
+        <v>146</v>
+      </c>
+      <c r="E676" s="9" t="s">
+        <v>845</v>
       </c>
       <c r="F676" s="9" t="s">
         <v>5</v>
@@ -21581,7 +21708,7 @@
     </row>
     <row r="677" spans="1:8" s="9" customFormat="1">
       <c r="A677" s="9" t="s">
-        <v>823</v>
+        <v>1613</v>
       </c>
       <c r="B677" s="9" t="s">
         <v>143</v>
@@ -21590,13 +21717,13 @@
         <v>145</v>
       </c>
       <c r="D677" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E677" s="9" t="s">
-        <v>845</v>
+        <v>1419</v>
       </c>
       <c r="F677" s="9" t="s">
         <v>5</v>
+      </c>
+      <c r="H677" s="9" t="s">
+        <v>1998</v>
       </c>
     </row>
     <row r="678" spans="1:8" s="9" customFormat="1">
@@ -22267,7 +22394,7 @@
   </sheetData>
   <sortState ref="A2:I709">
     <sortCondition ref="B2:B709"/>
-    <sortCondition ref="H2:H709"/>
+    <sortCondition ref="A2:A709"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -22281,29 +22408,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F77" sqref="F77"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" customWidth="1"/>
     <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18">
       <c r="A1" s="7" t="s">
         <v>570</v>
       </c>
@@ -22322,17 +22448,14 @@
       <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>1964</v>
+      <c r="G1" s="1" t="s">
+        <v>1962</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1962</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>1963</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1">
+    <row r="2" spans="1:8" s="8" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>823</v>
       </c>
@@ -22351,14 +22474,14 @@
       <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="8" t="s">
+        <v>1960</v>
+      </c>
       <c r="H2" s="8" t="s">
-        <v>1960</v>
-      </c>
-      <c r="I2" s="8" t="s">
         <v>1961</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="8" customFormat="1">
+    <row r="3" spans="1:8" s="8" customFormat="1">
       <c r="A3" s="8" t="s">
         <v>571</v>
       </c>
@@ -22377,14 +22500,14 @@
       <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="G3" s="8" t="s">
+        <v>1960</v>
+      </c>
       <c r="H3" s="8" t="s">
-        <v>1960</v>
-      </c>
-      <c r="I3" s="8" t="s">
         <v>1961</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>1958</v>
       </c>
@@ -22403,14 +22526,11 @@
       <c r="F4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>2001</v>
-      </c>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>1971</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1">
+    <row r="5" spans="1:8" s="8" customFormat="1">
       <c r="A5" s="8" t="s">
         <v>1127</v>
       </c>
@@ -22429,14 +22549,14 @@
       <c r="F5" s="8" t="s">
         <v>93</v>
       </c>
+      <c r="G5" s="8" t="s">
+        <v>2004</v>
+      </c>
       <c r="H5" s="8" t="s">
-        <v>2004</v>
-      </c>
-      <c r="I5" s="8" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="8" customFormat="1">
+    <row r="6" spans="1:8" s="8" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>823</v>
       </c>
@@ -22455,14 +22575,14 @@
       <c r="F6" s="8" t="s">
         <v>93</v>
       </c>
+      <c r="G6" s="8" t="s">
+        <v>2004</v>
+      </c>
       <c r="H6" s="8" t="s">
-        <v>2004</v>
-      </c>
-      <c r="I6" s="8" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1">
+    <row r="7" spans="1:8" s="8" customFormat="1">
       <c r="A7" s="8" t="s">
         <v>571</v>
       </c>
@@ -22481,227 +22601,209 @@
       <c r="F7" s="8" t="s">
         <v>93</v>
       </c>
+      <c r="G7" s="8" t="s">
+        <v>2004</v>
+      </c>
       <c r="H7" s="8" t="s">
-        <v>2004</v>
-      </c>
-      <c r="I7" s="8" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="9" customFormat="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:8" s="17" customFormat="1">
+      <c r="A8" s="17" t="s">
         <v>1958</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="17" t="s">
         <v>677</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="17" t="s">
         <v>1970</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="18" t="s">
         <v>1638</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="18" t="s">
         <v>1638</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2001</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="F8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>1969</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:8" s="17" customFormat="1">
+      <c r="A9" s="17" t="s">
         <v>1283</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="17" t="s">
         <v>677</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="17" t="s">
         <v>1970</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="17" t="s">
         <v>1187</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="17" t="s">
         <v>1242</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>2001</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="F9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>1968</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="9" customFormat="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:8" s="17" customFormat="1">
+      <c r="A10" s="17" t="s">
         <v>823</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="17" t="s">
         <v>677</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="17" t="s">
         <v>1970</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="17" t="s">
         <v>678</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="17" t="s">
         <v>863</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>2001</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="F10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>1968</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="9" customFormat="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:8" s="12" customFormat="1">
+      <c r="A11" s="12" t="s">
         <v>1283</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="16" t="s">
         <v>1210</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>2007</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="G11" s="12" t="s">
         <v>1972</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="9" customFormat="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:8" s="12" customFormat="1">
+      <c r="A12" s="12" t="s">
         <v>823</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="12" t="s">
         <v>859</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="9" customFormat="1">
-      <c r="A13" s="9" t="s">
+      <c r="F12" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="12" customFormat="1">
+      <c r="A13" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="9" customFormat="1">
-      <c r="A14" s="9" t="s">
+      <c r="F13" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="17" customFormat="1">
+      <c r="A14" s="17" t="s">
         <v>1283</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="17" t="s">
         <v>1202</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="F14" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>1973</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="9" customFormat="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:8" s="17" customFormat="1">
+      <c r="A15" s="17" t="s">
         <v>823</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="17" t="s">
         <v>899</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="9" customFormat="1">
-      <c r="A16" s="9" t="s">
+      <c r="F15" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="17" customFormat="1">
+      <c r="A16" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="9" customFormat="1">
+      <c r="F16" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
         <v>823</v>
       </c>
@@ -22720,17 +22822,14 @@
       <c r="F17" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>1974</v>
+      <c r="G17" s="8" t="s">
+        <v>1863</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>1863</v>
-      </c>
-      <c r="I17" s="8" t="s">
         <v>1751</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="9" customFormat="1">
+    <row r="18" spans="1:8" s="9" customFormat="1">
       <c r="A18" s="9" t="s">
         <v>571</v>
       </c>
@@ -22749,106 +22848,103 @@
       <c r="F18" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>1974</v>
+      <c r="G18" s="8" t="s">
+        <v>1863</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>1863</v>
-      </c>
-      <c r="I18" s="8" t="s">
         <v>1751</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:8" s="17" customFormat="1">
+      <c r="A19" s="17" t="s">
         <v>1127</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="17" t="s">
         <v>392</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="G19" s="17" t="s">
         <v>1975</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="9" customFormat="1">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:8" s="17" customFormat="1">
+      <c r="A20" s="17" t="s">
         <v>823</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="17" t="s">
         <v>392</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="G20" s="17" t="s">
         <v>1975</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="9" customFormat="1">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:8" s="17" customFormat="1">
+      <c r="A21" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="17" t="s">
         <v>392</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="G21" s="17" t="s">
         <v>1975</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="9" customFormat="1">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:8" s="17" customFormat="1">
+      <c r="A22" s="17" t="s">
         <v>1958</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="17" t="s">
         <v>392</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="18" t="s">
         <v>1639</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="18" t="s">
         <v>1639</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1">
+    <row r="23" spans="1:8" s="9" customFormat="1">
       <c r="A23" s="9" t="s">
         <v>1283</v>
       </c>
@@ -22867,11 +22963,11 @@
       <c r="F23" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>1978</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1">
+    <row r="24" spans="1:8" s="9" customFormat="1">
       <c r="A24" s="9" t="s">
         <v>571</v>
       </c>
@@ -22891,96 +22987,96 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="12" customFormat="1">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:8" s="17" customFormat="1">
+      <c r="A25" s="17" t="s">
         <v>1127</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="17" t="s">
         <v>766</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="17" t="s">
         <v>766</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="G25" s="17" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="12" customFormat="1">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:8" s="17" customFormat="1">
+      <c r="A26" s="17" t="s">
         <v>1283</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="17" t="s">
         <v>1169</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="17" t="s">
         <v>1169</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="G26" s="17" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="12" customFormat="1">
-      <c r="A27" s="12" t="s">
+    <row r="27" spans="1:8" s="17" customFormat="1">
+      <c r="A27" s="17" t="s">
         <v>823</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="17" t="s">
         <v>766</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="17" t="s">
         <v>766</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="G27" s="17" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="12" customFormat="1">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:8" s="17" customFormat="1">
+      <c r="A28" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="9" customFormat="1">
+    <row r="29" spans="1:8" s="9" customFormat="1">
       <c r="A29" s="9" t="s">
         <v>1127</v>
       </c>
@@ -22999,14 +23095,11 @@
       <c r="F29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>1965</v>
-      </c>
-      <c r="H29" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>1991</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="9" customFormat="1">
+    <row r="30" spans="1:8" s="9" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>1958</v>
       </c>
@@ -23025,14 +23118,11 @@
       <c r="F30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>1965</v>
-      </c>
-      <c r="H30" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>1991</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="9" customFormat="1">
+    <row r="31" spans="1:8" s="9" customFormat="1">
       <c r="A31" s="9" t="s">
         <v>571</v>
       </c>
@@ -23051,113 +23141,100 @@
       <c r="F31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>1965</v>
-      </c>
-      <c r="H31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>1992</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:8" s="17" customFormat="1">
+      <c r="A32" s="17" t="s">
         <v>1958</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="17" t="s">
         <v>594</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="17" t="s">
         <v>595</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="18" t="s">
         <v>1642</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="18" t="s">
         <v>1642</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>1966</v>
-      </c>
-      <c r="H32" s="3" t="s">
+      <c r="G32" s="17" t="s">
         <v>1979</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="3" customFormat="1">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:8" s="17" customFormat="1">
+      <c r="A33" s="17" t="s">
         <v>1127</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="17" t="s">
         <v>594</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="17" t="s">
         <v>595</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="17" t="s">
         <v>596</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="17" t="s">
         <v>949</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>1966</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="3" customFormat="1">
-      <c r="A34" s="3" t="s">
+      <c r="F33" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="17" customFormat="1">
+      <c r="A34" s="17" t="s">
         <v>823</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="17" t="s">
         <v>594</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="17" t="s">
         <v>595</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="17" t="s">
         <v>596</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="17" t="s">
         <v>830</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>1966</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="2" t="s">
+      <c r="F34" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="8" customFormat="1">
+      <c r="A35" s="8" t="s">
         <v>823</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="8" t="s">
         <v>797</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="8" t="s">
         <v>798</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="8" t="s">
         <v>799</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="8" t="s">
         <v>922</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="2"/>
+      <c r="F35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>2024</v>
+      </c>
       <c r="H35" s="8" t="s">
-        <v>2026</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="3" customFormat="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="3" customFormat="1">
       <c r="A36" s="3" t="s">
         <v>1958</v>
       </c>
@@ -23176,17 +23253,14 @@
       <c r="F36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>1980</v>
+      <c r="G36" s="8" t="s">
+        <v>2022</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>2024</v>
-      </c>
-      <c r="I36" s="8" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="3" customFormat="1">
+    <row r="37" spans="1:8" s="3" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>823</v>
       </c>
@@ -23205,17 +23279,14 @@
       <c r="F37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>1980</v>
+      <c r="G37" s="8" t="s">
+        <v>2022</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>2024</v>
-      </c>
-      <c r="I37" s="8" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="3" customFormat="1">
+    <row r="38" spans="1:8" s="3" customFormat="1">
       <c r="A38" s="3" t="s">
         <v>1613</v>
       </c>
@@ -23231,60 +23302,57 @@
       <c r="F38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="8" t="s">
+        <v>2022</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="17" customFormat="1">
+      <c r="A39" s="17" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" s="17" t="s">
         <v>1980</v>
       </c>
-      <c r="H38" s="8" t="s">
-        <v>2024</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="14" customFormat="1">
-      <c r="A39" s="14" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B39" s="14" t="s">
+    </row>
+    <row r="40" spans="1:8" s="17" customFormat="1">
+      <c r="A40" s="17" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>1272</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C40" s="17" t="s">
         <v>1263</v>
       </c>
-      <c r="D39" s="15" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>1185</v>
-      </c>
-      <c r="F39" s="14" t="s">
+      <c r="D40" s="17" t="s">
+        <v>1598</v>
+      </c>
+      <c r="F40" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="G40" s="17" t="s">
         <v>1980</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="14" customFormat="1">
-      <c r="A40" s="14" t="s">
-        <v>1613</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>1263</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>1598</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="14" customFormat="1">
+    <row r="41" spans="1:8" s="14" customFormat="1">
       <c r="A41" s="14" t="s">
         <v>1283</v>
       </c>
@@ -23303,11 +23371,11 @@
       <c r="F41" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="14" t="s">
+      <c r="G41" s="14" t="s">
         <v>1993</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="14" customFormat="1">
+    <row r="42" spans="1:8" s="14" customFormat="1">
       <c r="A42" s="14" t="s">
         <v>1613</v>
       </c>
@@ -23323,54 +23391,54 @@
       <c r="F42" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="G42" s="14" t="s">
         <v>1993</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="12" customFormat="1">
-      <c r="A43" s="12" t="s">
+    <row r="43" spans="1:8" s="17" customFormat="1">
+      <c r="A43" s="17" t="s">
         <v>1283</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="17" t="s">
         <v>1266</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="17" t="s">
         <v>1258</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="17" t="s">
         <v>1152</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="17" t="s">
         <v>1218</v>
       </c>
-      <c r="F43" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H43" s="12" t="s">
+      <c r="F43" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="17" t="s">
         <v>1994</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="12" customFormat="1">
-      <c r="A44" s="12" t="s">
+    <row r="44" spans="1:8" s="17" customFormat="1">
+      <c r="A44" s="17" t="s">
         <v>1958</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="17" t="s">
         <v>1266</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="17" t="s">
         <v>1258</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="18" t="s">
         <v>1646</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="18" t="s">
         <v>1646</v>
       </c>
-      <c r="F44" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="14" customFormat="1">
+      <c r="F44" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="14" customFormat="1">
       <c r="A45" s="14" t="s">
         <v>1283</v>
       </c>
@@ -23389,11 +23457,11 @@
       <c r="F45" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H45" s="15" t="s">
+      <c r="G45" s="15" t="s">
         <v>1647</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="14" customFormat="1">
+    <row r="46" spans="1:8" s="14" customFormat="1">
       <c r="A46" s="14" t="s">
         <v>1958</v>
       </c>
@@ -23413,88 +23481,92 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:8" s="17" customFormat="1">
+      <c r="A47" s="17" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>1648</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>1648</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="17" customFormat="1">
+      <c r="A48" s="17" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="17" customFormat="1">
+      <c r="A49" s="17" t="s">
         <v>1613</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>1479</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" s="14" customFormat="1">
-      <c r="A48" s="14" t="s">
-        <v>1958</v>
-      </c>
-      <c r="B48" s="14" t="s">
+      <c r="B49" s="17" t="s">
         <v>1252</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C49" s="17" t="s">
         <v>1285</v>
       </c>
-      <c r="D48" s="15" t="s">
-        <v>1648</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>1648</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="14" customFormat="1">
-      <c r="A49" s="14" t="s">
+      <c r="D49" s="17" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="14" customFormat="1">
+      <c r="A50" s="14" t="s">
         <v>1283</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>1285</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>1205</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="14" customFormat="1">
-      <c r="A50" s="14" t="s">
+      <c r="B50" s="14" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="14" customFormat="1">
+      <c r="A51" s="14" t="s">
         <v>1613</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>1285</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="14" customFormat="1">
-      <c r="A51" s="14" t="s">
-        <v>1283</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>1281</v>
@@ -23503,144 +23575,144 @@
         <v>1250</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>1135</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>1135</v>
+        <v>1363</v>
       </c>
       <c r="F51" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H51" s="14" t="s">
+      <c r="G51" s="14" t="s">
         <v>1980</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="14" customFormat="1">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="1:7" s="17" customFormat="1">
+      <c r="A52" s="17" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>1649</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="17" customFormat="1">
+      <c r="A53" s="17" t="s">
         <v>1613</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>1281</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>1250</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>1363</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="12" customFormat="1">
-      <c r="A53" s="12" t="s">
-        <v>1958</v>
-      </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="D53" s="16" t="s">
-        <v>1649</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>1649</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H53" s="12" t="s">
+      <c r="D53" s="17" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="17" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="12" customFormat="1">
-      <c r="A54" s="12" t="s">
-        <v>1613</v>
-      </c>
-      <c r="B54" s="12" t="s">
+    <row r="54" spans="1:7" s="17" customFormat="1">
+      <c r="A54" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B54" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>1400</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H54" s="12" t="s">
+      <c r="D54" s="17" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" s="12" customFormat="1">
-      <c r="A55" s="12" t="s">
+      <c r="E54" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="17" customFormat="1">
+      <c r="A55" s="17" t="s">
+        <v>823</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>837</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="17" customFormat="1">
+      <c r="A56" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="12" customFormat="1">
+      <c r="A57" s="12" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="12" customFormat="1">
+      <c r="A58" s="12" t="s">
         <v>1127</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="12" customFormat="1">
-      <c r="A56" s="12" t="s">
-        <v>823</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>837</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="12" customFormat="1">
-      <c r="A57" s="12" t="s">
-        <v>571</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="12" customFormat="1">
-      <c r="A58" s="12" t="s">
-        <v>1283</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>90</v>
@@ -23649,21 +23721,18 @@
         <v>92</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>1165</v>
+        <v>91</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>1165</v>
+        <v>91</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H58" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="12" customFormat="1">
+    </row>
+    <row r="59" spans="1:7" s="12" customFormat="1">
       <c r="A59" s="12" t="s">
-        <v>1127</v>
+        <v>823</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>90</v>
@@ -23681,9 +23750,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="12" customFormat="1">
+    <row r="60" spans="1:7" s="12" customFormat="1">
       <c r="A60" s="12" t="s">
-        <v>823</v>
+        <v>571</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>90</v>
@@ -23701,135 +23770,135 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="12" customFormat="1">
+    <row r="61" spans="1:7" s="3" customFormat="1">
       <c r="A61" s="12" t="s">
-        <v>571</v>
+        <v>1958</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>90</v>
+        <v>1862</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>91</v>
+        <v>1650</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>1650</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" s="3" customFormat="1">
-      <c r="A62" s="3" t="s">
+      <c r="G61" s="3" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="17" customFormat="1">
+      <c r="A62" s="17" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="17" customFormat="1">
+      <c r="A63" s="17" t="s">
         <v>1958</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>1862</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>1650</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>1650</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>1650</v>
-      </c>
-      <c r="F62" s="3" t="s">
+      <c r="B63" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F63" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>1997</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="14" customFormat="1">
-      <c r="A63" s="14" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B63" s="14" t="s">
+    </row>
+    <row r="64" spans="1:7" s="17" customFormat="1">
+      <c r="A64" s="17" t="s">
+        <v>823</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>431</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C64" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>1996</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="14" customFormat="1">
-      <c r="A64" s="14" t="s">
-        <v>1958</v>
-      </c>
-      <c r="B64" s="14" t="s">
+      <c r="D64" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="17" customFormat="1">
+      <c r="A65" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>431</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C65" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D65" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E65" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F65" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="14" customFormat="1">
-      <c r="A65" s="14" t="s">
-        <v>823</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>431</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="14" customFormat="1">
-      <c r="A66" s="14" t="s">
-        <v>571</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>431</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="F66" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" s="9" customFormat="1">
+    <row r="66" spans="1:7" s="9" customFormat="1">
+      <c r="A66" s="9" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" s="9" customFormat="1">
       <c r="A67" s="9" t="s">
-        <v>1613</v>
+        <v>1127</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>143</v>
@@ -23838,18 +23907,18 @@
         <v>145</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>1419</v>
+        <v>146</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="9" t="s">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" s="9" customFormat="1">
+    </row>
+    <row r="68" spans="1:7" s="9" customFormat="1">
       <c r="A68" s="9" t="s">
-        <v>1127</v>
+        <v>1958</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>143</v>
@@ -23857,19 +23926,19 @@
       <c r="C68" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="E68" s="10" t="s">
         <v>146</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="9" customFormat="1">
+    <row r="69" spans="1:7" s="9" customFormat="1">
       <c r="A69" s="9" t="s">
-        <v>1958</v>
+        <v>1283</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>143</v>
@@ -23877,19 +23946,19 @@
       <c r="C69" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>146</v>
+      <c r="D69" s="9" t="s">
+        <v>1150</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>146</v>
+        <v>1217</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="9" customFormat="1">
+    <row r="70" spans="1:7" s="9" customFormat="1">
       <c r="A70" s="9" t="s">
-        <v>1283</v>
+        <v>823</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>143</v>
@@ -23898,18 +23967,18 @@
         <v>145</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>1217</v>
+        <v>146</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>845</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="9" customFormat="1">
+    <row r="71" spans="1:7" s="9" customFormat="1">
       <c r="A71" s="9" t="s">
-        <v>823</v>
+        <v>571</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>143</v>
@@ -23921,29 +23990,9 @@
         <v>146</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>845</v>
+        <v>144</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="9" customFormat="1">
-      <c r="A72" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F72" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -23991,4 +24040,1370 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C120" sqref="C120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="8" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:4" s="8" customFormat="1">
+      <c r="A24" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="2" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1985</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="9" t="s">
+        <v>677</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="2" customFormat="1">
+      <c r="A43" s="2" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4" s="2" customFormat="1">
+      <c r="A44" s="2" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D65" s="9"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D66" s="9"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D67" s="9"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D71" s="9"/>
+    </row>
+    <row r="72" spans="1:4" s="8" customFormat="1">
+      <c r="A72" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="D72" s="9"/>
+    </row>
+    <row r="73" spans="1:4" s="8" customFormat="1">
+      <c r="A73" s="2" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" s="8" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="2" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="2" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="2" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D78" s="9"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="2" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D79" s="9"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="2" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D80" s="9"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="2" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="2" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="2" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="2" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="2" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="2" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="2" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="9" customFormat="1">
+      <c r="A91" s="2" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D91"/>
+    </row>
+    <row r="92" spans="1:4" s="9" customFormat="1">
+      <c r="A92" s="2" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="1:4" s="9" customFormat="1">
+      <c r="A93" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="D93"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="9" customFormat="1">
+      <c r="A98" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D98"/>
+    </row>
+    <row r="99" spans="1:4" s="9" customFormat="1">
+      <c r="A99" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D99"/>
+    </row>
+    <row r="100" spans="1:4" s="9" customFormat="1">
+      <c r="A100" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D100"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="9" customFormat="1">
+      <c r="A108" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D108"/>
+    </row>
+    <row r="109" spans="1:4" s="9" customFormat="1">
+      <c r="A109" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D109"/>
+    </row>
+    <row r="110" spans="1:4" s="9" customFormat="1">
+      <c r="A110" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D110"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="2" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="2" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:I709">
+    <sortCondition ref="C2:C709"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add information submitted to OMRSE
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@83109 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ClinEpi_metadata.xlsx
+++ b/Load/src/ontology/ClinEpi_metadata.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="4500" windowWidth="29420" windowHeight="13800" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1920" yWindow="3280" windowWidth="30320" windowHeight="14260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="terms" sheetId="1" r:id="rId1"/>
     <sheet name="issues" sheetId="3" r:id="rId2"/>
     <sheet name="notes" sheetId="2" r:id="rId3"/>
     <sheet name="term request" sheetId="4" r:id="rId4"/>
+    <sheet name="omrse" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5173" uniqueCount="2035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5287" uniqueCount="2080">
   <si>
     <t>ID</t>
   </si>
@@ -6127,13 +6128,148 @@
   </si>
   <si>
     <t>https://github.com/OHMI-ontology/OHMI/issues/1</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>An information content entity that is about human traveling.</t>
+  </si>
+  <si>
+    <t>An information content entity that is about employment.</t>
+  </si>
+  <si>
+    <t>An information content entity that is about the highest level of schooling that a person has reached.</t>
+  </si>
+  <si>
+    <t>an activity in which one engages An information content entity that is about something people are occupied with and you're not necessarily doing it to exchange for payment.</t>
+  </si>
+  <si>
+    <t>A data item of salary of primary job.</t>
+  </si>
+  <si>
+    <t>A data item of salary of other job.</t>
+  </si>
+  <si>
+    <t>A data item of income level issued annually by the Department of Health and Human Services. Federal poverty levels are used to determine your eligibility for certain programs and benefits.</t>
+  </si>
+  <si>
+    <t>A symbol that denotes a specific family, rather than the physical home in which they live.</t>
+  </si>
+  <si>
+    <t>An information content entity about items that a household owns such as a car, funiture, etc.</t>
+  </si>
+  <si>
+    <t>parent iD</t>
+  </si>
+  <si>
+    <t>parent label</t>
+  </si>
+  <si>
+    <t>IAO_0000030</t>
+  </si>
+  <si>
+    <t>EUPATH_0000353</t>
+  </si>
+  <si>
+    <t>IAO_0000027</t>
+  </si>
+  <si>
+    <t>IAO_0000416</t>
+  </si>
+  <si>
+    <t>IAO_0000028</t>
+  </si>
+  <si>
+    <t>information content entity</t>
+  </si>
+  <si>
+    <t>economic activity</t>
+  </si>
+  <si>
+    <t>data item</t>
+  </si>
+  <si>
+    <t>time measurement datum</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0004950</t>
+  </si>
+  <si>
+    <t>household wealth index</t>
+  </si>
+  <si>
+    <t>household assets</t>
+  </si>
+  <si>
+    <t>family income</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>employment</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>number of hours per day of employment</t>
+  </si>
+  <si>
+    <t>A planned process that a person participates in exchange for payment. The job role born by the person is realized in the process.</t>
+  </si>
+  <si>
+    <t>EUPATH_0000352</t>
+  </si>
+  <si>
+    <t>A human social role realized in a process that often performed in exchange for payment. Many people have multiple job roles, such as those of parent, homemaker, and employee.</t>
+  </si>
+  <si>
+    <t>job role</t>
+  </si>
+  <si>
+    <t>planned process</t>
+  </si>
+  <si>
+    <t>OMRSE_00000001</t>
+  </si>
+  <si>
+    <t>human social role</t>
+  </si>
+  <si>
+    <t>OBI_0000011</t>
+  </si>
+  <si>
+    <t>A data item of a household's cumulative living standard represented in a numerical datum. The wealth index is calculated using easy-to-collect data on a household's ownership of selected assets, such as televisions and bicycles; materials used for housing construction; and types of water access and sanitation facilities.</t>
+  </si>
+  <si>
+    <t>A data item about a household's cumulative living standard represented in a categorical datum. The wealth index is calculated using data on a household's ownership of selected assets, such as televisions and bicycles; materials used for housing construction; and types of water access and sanitation facilities.</t>
+  </si>
+  <si>
+    <t>A time measurement datum about number of hours per day spend at economic activity.</t>
+  </si>
+  <si>
+    <t>number of hours per day at economic activity</t>
+  </si>
+  <si>
+    <t>A symbol that denotes a specific household.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6216,6 +6352,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6234,7 +6377,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="357">
+  <cellStyleXfs count="421">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6592,8 +6735,72 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6615,8 +6822,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="357">
+  <cellStyles count="421">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6795,6 +7003,60 @@
     <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6973,6 +7235,16 @@
     <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7304,11 +7576,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I709"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C706" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G568" sqref="G568"/>
+      <selection pane="bottomRight" activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8366,76 +8638,94 @@
       </c>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="1:9" s="8" customFormat="1">
+      <c r="A49" s="8" t="s">
         <v>1127</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="8" t="s">
         <v>977</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="8" t="s">
         <v>977</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" s="2" t="s">
+      <c r="F49" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>2001</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="2" t="s">
+      <c r="H49" s="8" t="s">
+        <v>2058</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="8" customFormat="1">
+      <c r="A50" s="8" t="s">
         <v>1283</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="8" t="s">
         <v>1139</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="8" t="s">
         <v>1207</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="2" t="s">
+      <c r="F50" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>2001</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="2" t="s">
+      <c r="H50" s="8" t="s">
+        <v>2058</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="8" customFormat="1">
+      <c r="A51" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="2" t="s">
+      <c r="F51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>2001</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="8" t="s">
+        <v>2058</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="2" t="s">
         <v>823</v>
       </c>
@@ -8456,7 +8746,7 @@
       </c>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:9">
       <c r="A53" s="2" t="s">
         <v>571</v>
       </c>
@@ -8477,7 +8767,7 @@
       </c>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:9">
       <c r="A54" s="2" t="s">
         <v>571</v>
       </c>
@@ -8498,7 +8788,7 @@
       </c>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:9">
       <c r="A55" s="2" t="s">
         <v>571</v>
       </c>
@@ -8519,7 +8809,7 @@
       </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
         <v>571</v>
       </c>
@@ -8540,7 +8830,7 @@
       </c>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:9">
       <c r="A57" s="2" t="s">
         <v>823</v>
       </c>
@@ -8561,7 +8851,7 @@
       </c>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:9">
       <c r="A58" s="2" t="s">
         <v>571</v>
       </c>
@@ -8582,7 +8872,7 @@
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:9">
       <c r="A59" s="2" t="s">
         <v>571</v>
       </c>
@@ -8603,7 +8893,7 @@
       </c>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:9">
       <c r="A60" s="2" t="s">
         <v>823</v>
       </c>
@@ -8624,7 +8914,7 @@
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:9">
       <c r="A61" s="2" t="s">
         <v>571</v>
       </c>
@@ -8645,7 +8935,7 @@
       </c>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:9">
       <c r="A62" s="2" t="s">
         <v>1958</v>
       </c>
@@ -8668,7 +8958,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:9">
       <c r="A63" s="2" t="s">
         <v>1283</v>
       </c>
@@ -8691,7 +8981,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:9">
       <c r="A64" s="2" t="s">
         <v>823</v>
       </c>
@@ -24046,11 +24336,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C120" sqref="C120"/>
+      <selection pane="bottomRight" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25406,4 +25696,402 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="C1" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2046</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2047</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B3" t="s">
+        <v>607</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="9" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2064</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" s="9" customFormat="1">
+      <c r="A5" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B6" t="s">
+        <v>792</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2051</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="9" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" s="9" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B11" t="s">
+        <v>627</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2043</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2060</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1550</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>2049</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2054</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2074</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2072</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2073</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2059</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2059</v>
+      </c>
+      <c r="C18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add two variables in PRISM ontology
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@83299 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ClinEpi_metadata.xlsx
+++ b/Load/src/ontology/ClinEpi_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19340" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="540" windowWidth="25040" windowHeight="13640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="terms" sheetId="1" r:id="rId1"/>
@@ -7025,12 +7025,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -7042,7 +7048,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="463">
+  <cellStyleXfs count="479">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7506,8 +7512,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7531,8 +7553,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="463">
+  <cellStyles count="479">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7786,6 +7809,14 @@
     <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7995,6 +8026,14 @@
     <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8327,10 +8366,10 @@
   <dimension ref="A1:J709"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D538" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C665" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I597" sqref="I597"/>
+      <selection pane="bottomRight" activeCell="C672" sqref="C672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22978,8 +23017,8 @@
       <c r="C675" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D675" s="9" t="s">
-        <v>146</v>
+      <c r="D675" s="21" t="s">
+        <v>1217</v>
       </c>
       <c r="E675" s="9" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
add harmonization issue sheet
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@83307 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ClinEpi_metadata.xlsx
+++ b/Load/src/ontology/ClinEpi_metadata.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="540" windowWidth="25040" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="3140" windowWidth="29840" windowHeight="15660" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="terms" sheetId="1" r:id="rId1"/>
-    <sheet name="issues" sheetId="3" r:id="rId2"/>
-    <sheet name="notes" sheetId="2" r:id="rId3"/>
-    <sheet name="term request" sheetId="4" r:id="rId4"/>
-    <sheet name="omrse" sheetId="5" r:id="rId5"/>
-    <sheet name="values" sheetId="6" r:id="rId6"/>
+    <sheet name="discussion" sheetId="7" r:id="rId1"/>
+    <sheet name="terms" sheetId="1" r:id="rId2"/>
+    <sheet name="issues" sheetId="3" r:id="rId3"/>
+    <sheet name="notes" sheetId="2" r:id="rId4"/>
+    <sheet name="term request" sheetId="4" r:id="rId5"/>
+    <sheet name="omrse" sheetId="5" r:id="rId6"/>
+    <sheet name="values" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5905" uniqueCount="2299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6245" uniqueCount="2311">
   <si>
     <t>ID</t>
   </si>
@@ -6921,6 +6922,42 @@
   </si>
   <si>
     <t>deleted</t>
+  </si>
+  <si>
+    <t>change to febrile? Or since it is a category rather than search qualifier, shall we add a new ontology term?</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Same ontology term with different display names in different projects including:</t>
+  </si>
+  <si>
+    <t>Gates project (variables from HBDG)</t>
+  </si>
+  <si>
+    <t>Uganda ICEMR project</t>
+  </si>
+  <si>
+    <t>ICEMR protein array data collected from different ICEMR centers, website: http://plasmodb.org/plasmo/showQuestion.do?questionFullName=InternalGeneDatasetQuestions.GenesByProteinArray#GeneQuestions.GenesByICEMRHostResponse</t>
+  </si>
+  <si>
+    <t>Amazonia ICEMR project, inactive now</t>
+  </si>
+  <si>
+    <t>Indian ICEMR project, inactive now</t>
+  </si>
+  <si>
+    <t>change to "Village"?</t>
+  </si>
+  <si>
+    <t>collection date?</t>
+  </si>
+  <si>
+    <t>Shall we change it to 'Gender'?</t>
+  </si>
+  <si>
+    <t>shall we change it to laboratory findings? Or change laboratory finds to laboratory test? Question need to be discussed between Chris and Jie</t>
   </si>
 </sst>
 </file>
@@ -7025,7 +7062,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7035,6 +7072,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7048,7 +7091,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="479">
+  <cellStyleXfs count="501">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7528,8 +7571,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7554,8 +7619,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="479">
+  <cellStyles count="501">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7817,6 +7884,17 @@
     <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -8034,6 +8112,17 @@
     <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8363,13 +8452,1219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>571</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="18">
+      <c r="A9" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>1638</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1">
+      <c r="A12" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>678</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1"/>
+    <row r="14" spans="1:6" s="2" customFormat="1">
+      <c r="A14" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1">
+      <c r="A15" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1">
+      <c r="A16" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1"/>
+    <row r="18" spans="1:6" s="2" customFormat="1">
+      <c r="A18" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1">
+      <c r="A19" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1">
+      <c r="A20" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1"/>
+    <row r="22" spans="1:6" s="2" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1"/>
+    <row r="25" spans="1:6" s="2" customFormat="1">
+      <c r="A25" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>766</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1">
+      <c r="A26" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1">
+      <c r="A27" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>766</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1">
+      <c r="A28" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1"/>
+    <row r="30" spans="1:6" s="2" customFormat="1">
+      <c r="A30" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1">
+      <c r="A32" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1"/>
+    <row r="34" spans="1:6" s="2" customFormat="1">
+      <c r="A34" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>1642</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1">
+      <c r="A35" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1">
+      <c r="A36" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1"/>
+    <row r="38" spans="1:6" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1">
+      <c r="A39" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>796</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1">
+      <c r="A40" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>1612</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1"/>
+    <row r="42" spans="1:6" s="2" customFormat="1">
+      <c r="A42" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1">
+      <c r="A43" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1"/>
+    <row r="45" spans="1:6" s="2" customFormat="1">
+      <c r="A45" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>2308</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1">
+      <c r="A46" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1">
+      <c r="A47" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="2" customFormat="1"/>
+    <row r="49" spans="1:6" s="2" customFormat="1">
+      <c r="A49" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="2" customFormat="1">
+      <c r="A50" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>1646</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="2" customFormat="1">
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" s="2" customFormat="1">
+      <c r="A52" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="2" customFormat="1">
+      <c r="A53" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="2" customFormat="1">
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" s="2" customFormat="1">
+      <c r="A55" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>1648</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="2" customFormat="1">
+      <c r="A56" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1">
+      <c r="A57" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="2" customFormat="1"/>
+    <row r="59" spans="1:6" s="2" customFormat="1">
+      <c r="A59" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="2" customFormat="1">
+      <c r="A60" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="2" customFormat="1"/>
+    <row r="62" spans="1:6" s="2" customFormat="1">
+      <c r="A62" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="2" customFormat="1">
+      <c r="A63" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="2" customFormat="1">
+      <c r="A64" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="2" customFormat="1">
+      <c r="A65" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="2" customFormat="1">
+      <c r="A66" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="2" customFormat="1"/>
+    <row r="68" spans="1:6" s="2" customFormat="1">
+      <c r="A68" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="2" customFormat="1">
+      <c r="A69" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="2" customFormat="1">
+      <c r="A70" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="2" customFormat="1">
+      <c r="A71" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="2" customFormat="1">
+      <c r="A72" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>1650</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="2" customFormat="1">
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" s="2" customFormat="1">
+      <c r="A74" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="2" customFormat="1">
+      <c r="A75" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="2" customFormat="1">
+      <c r="A76" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="2" customFormat="1">
+      <c r="A77" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="2" customFormat="1"/>
+    <row r="79" spans="1:6" s="2" customFormat="1">
+      <c r="A79" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="2" customFormat="1">
+      <c r="A80" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="2" customFormat="1">
+      <c r="A81" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="2" customFormat="1">
+      <c r="A82" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="2" customFormat="1">
+      <c r="A83" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="2" customFormat="1">
+      <c r="A84" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D84" s="22" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J709"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C665" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C459" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C672" sqref="C672"/>
+      <selection pane="bottomRight" activeCell="B470" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23770,7 +25065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
@@ -25371,7 +26666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -25406,7 +26701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D122"/>
   <sheetViews>
@@ -26772,7 +28067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
@@ -27170,7 +28465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>

</xml_diff>